<commit_message>
JUL update, lab foundation
</commit_message>
<xml_diff>
--- a/data/Publication details.xlsx
+++ b/data/Publication details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conorisco/Dropbox (Personal)/Jobs/CV and Publications/CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64383AB2-9F1C-E042-8743-1B48EF679862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584A4ED1-C1EA-8740-8D35-AE4845A483B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2500" windowWidth="32100" windowHeight="18620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Total papers</t>
   </si>
   <si>
-    <t>As corresponding author</t>
-  </si>
-  <si>
     <t xml:space="preserve">As First Author </t>
   </si>
   <si>
@@ -48,10 +45,10 @@
     <t>Seconday author - Major contribution  (&gt;3 months)</t>
   </si>
   <si>
-    <t>Papers in review as Co-First/Final author</t>
-  </si>
-  <si>
     <t>Senior, Co-senior or primary supervisor</t>
+  </si>
+  <si>
+    <t>As (co-)corresponding author</t>
   </si>
 </sst>
 </file>
@@ -369,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -383,10 +380,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -394,12 +391,12 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -407,15 +404,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -423,7 +420,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -431,18 +428,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>